<commit_message>
add a new pallets specs table and related web pages.
</commit_message>
<xml_diff>
--- a/public/BAF_BAXXX_1212_1212_.xlsx
+++ b/public/BAF_BAXXX_1212_1212_.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
   <si>
     <t>2948 Barossa Valley Way, Tanunda SA 5352</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Ph: (08) 8563 3046  Fax: (08) 8563 3643  Email: admin@barossatrading.com</t>
   </si>
   <si>
-    <t>BA132</t>
+    <t>BA161</t>
   </si>
   <si>
     <t>BOTTLING APPROVAL FORM    (BAF)</t>
@@ -119,7 +119,7 @@
     <t>Exact Cases</t>
   </si>
   <si>
-    <t>Req'd by:</t>
+    <t>Required By:</t>
   </si>
   <si>
     <t>11/11/1111</t>
@@ -128,6 +128,9 @@
     <t>Total Cases</t>
   </si>
   <si>
+    <t>Delivered By:</t>
+  </si>
+  <si>
     <t>22/02/2212</t>
   </si>
   <si>
@@ -279,6 +282,9 @@
   </si>
   <si>
     <t xml:space="preserve">Label </t>
+  </si>
+  <si>
+    <t>CS FR+BK</t>
   </si>
   <si>
     <t>Carton</t>
@@ -1187,7 +1193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="190">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -1472,9 +1478,6 @@
       <protection locked="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="14" fillId="0" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="8" numFmtId="0" fillId="0" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
@@ -1639,18 +1642,6 @@
     <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="16" numFmtId="1" fillId="0" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="16" numFmtId="0" fillId="0" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
-    <xf xfId="0" fontId="16" numFmtId="0" fillId="0" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
-    </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -1772,6 +1763,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="46" numFmtId="0" fillId="0" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="1" fillId="0" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -2155,7 +2152,7 @@
   <dimension ref="A1:AG123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="D39" sqref="D39:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.81640625" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2238,10 +2235,10 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="I4" s="19"/>
-      <c r="J4" s="188" t="s">
+      <c r="J4" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="188"/>
+      <c r="K4" s="184"/>
       <c r="L4" s="19"/>
       <c r="M4" s="17"/>
       <c r="N4" s="20"/>
@@ -2257,12 +2254,12 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="190">
+      <c r="H5" s="186">
         <v>1212</v>
       </c>
-      <c r="I5" s="190"/>
-      <c r="J5" s="189"/>
-      <c r="K5" s="189"/>
+      <c r="I5" s="186"/>
+      <c r="J5" s="185"/>
+      <c r="K5" s="185"/>
       <c r="L5" s="19"/>
       <c r="M5" s="17"/>
       <c r="N5" s="20"/>
@@ -2270,10 +2267,10 @@
       <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:33" customHeight="1" ht="14.25">
-      <c r="A6" s="166" t="s">
+      <c r="A6" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="166"/>
+      <c r="B6" s="162"/>
       <c r="C6" s="23" t="s">
         <v>7</v>
       </c>
@@ -2283,8 +2280,8 @@
       <c r="G6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="191"/>
-      <c r="I6" s="191"/>
+      <c r="H6" s="187"/>
+      <c r="I6" s="187"/>
       <c r="J6" s="26" t="s">
         <v>9</v>
       </c>
@@ -2302,10 +2299,10 @@
       </c>
     </row>
     <row r="7" spans="1:33" customHeight="1" ht="14.5">
-      <c r="A7" s="166" t="s">
+      <c r="A7" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="166"/>
+      <c r="B7" s="162"/>
       <c r="C7" s="23" t="s">
         <v>15</v>
       </c>
@@ -2320,10 +2317,10 @@
       <c r="O7" s="32"/>
     </row>
     <row r="8" spans="1:33" customHeight="1" ht="13.5">
-      <c r="A8" s="166" t="s">
+      <c r="A8" s="162" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="166"/>
+      <c r="B8" s="162"/>
       <c r="C8" s="33" t="s">
         <v>17</v>
       </c>
@@ -2345,10 +2342,10 @@
       <c r="O8" s="32"/>
     </row>
     <row r="9" spans="1:33" customHeight="1" ht="13">
-      <c r="A9" s="166" t="s">
+      <c r="A9" s="162" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="166"/>
+      <c r="B9" s="162"/>
       <c r="C9" s="36" t="s">
         <v>20</v>
       </c>
@@ -2376,10 +2373,10 @@
       <c r="O10" s="32"/>
     </row>
     <row r="11" spans="1:33" customHeight="1" ht="13.5">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="162" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="166"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="39" t="s">
         <v>23</v>
       </c>
@@ -2424,10 +2421,10 @@
       <c r="O13" s="32"/>
     </row>
     <row r="14" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A14" s="166" t="s">
+      <c r="A14" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="175"/>
+      <c r="B14" s="171"/>
       <c r="C14" s="44">
         <v>50001</v>
       </c>
@@ -2448,21 +2445,21 @@
       <c r="O14" s="32"/>
     </row>
     <row r="15" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A15" s="166" t="s">
+      <c r="A15" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="175"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="48">
         <v>1</v>
       </c>
       <c r="D15" s="49"/>
-      <c r="E15" s="182" t="s">
+      <c r="E15" s="178" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="184" t="s">
+      <c r="F15" s="180" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="185"/>
+      <c r="G15" s="181"/>
       <c r="H15" s="50" t="s">
         <v>33</v>
       </c>
@@ -2476,21 +2473,20 @@
       <c r="O15" s="32"/>
     </row>
     <row r="16" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A16" s="166" t="s">
+      <c r="A16" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="175"/>
-      <c r="C16" s="48">
-        <f>C14+C15</f>
-        <v>50002</v>
-      </c>
+      <c r="B16" s="171"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="49"/>
-      <c r="E16" s="183"/>
-      <c r="F16" s="186"/>
-      <c r="G16" s="187"/>
-      <c r="H16" s="51"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="182"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="51" t="s">
+        <v>36</v>
+      </c>
       <c r="I16" s="52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J16" s="42"/>
       <c r="K16" s="42"/>
@@ -2499,27 +2495,24 @@
       <c r="O16" s="32"/>
     </row>
     <row r="17" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A17" s="166" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="175"/>
-      <c r="C17" s="53">
-        <f>C16*M37</f>
-        <v>227509.1</v>
-      </c>
+      <c r="A17" s="162" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="171"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="54"/>
       <c r="E17" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="177"/>
+      <c r="F17" s="172" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="173"/>
       <c r="H17" s="55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I17" s="56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J17" s="42"/>
       <c r="K17" s="42"/>
@@ -2528,21 +2521,21 @@
       <c r="O17" s="32"/>
     </row>
     <row r="18" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A18" s="166" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="175"/>
+      <c r="A18" s="162" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="171"/>
       <c r="C18" s="57"/>
       <c r="D18" s="58"/>
       <c r="E18" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="178" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="179"/>
+        <v>44</v>
+      </c>
+      <c r="F18" s="174" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="175"/>
       <c r="H18" s="59" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I18" s="60">
         <v>2</v>
@@ -2554,21 +2547,21 @@
       <c r="O18" s="32"/>
     </row>
     <row r="19" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A19" s="166" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="175"/>
+      <c r="A19" s="162" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="171"/>
       <c r="C19" s="57"/>
       <c r="D19" s="49"/>
       <c r="E19" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="180">
+        <v>47</v>
+      </c>
+      <c r="F19" s="176">
         <v>12.0</v>
       </c>
-      <c r="G19" s="181"/>
+      <c r="G19" s="177"/>
       <c r="H19" s="59" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I19" s="60">
         <v>1</v>
@@ -2580,23 +2573,23 @@
       <c r="O19" s="32"/>
     </row>
     <row r="20" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A20" s="166" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="166"/>
+      <c r="A20" s="162" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="162"/>
       <c r="C20" s="62" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="167">
+        <v>50</v>
+      </c>
+      <c r="F20" s="163">
         <v>12.0</v>
       </c>
-      <c r="G20" s="168"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="172"/>
+      <c r="G20" s="164"/>
+      <c r="H20" s="167"/>
+      <c r="I20" s="168"/>
       <c r="J20" s="63"/>
       <c r="K20" s="63"/>
       <c r="M20" s="32"/>
@@ -2604,23 +2597,23 @@
       <c r="O20" s="32"/>
     </row>
     <row r="21" spans="1:33" customHeight="1" ht="17.15">
-      <c r="A21" s="166" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="166"/>
+      <c r="A21" s="162" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="162"/>
       <c r="C21" s="62" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="58"/>
       <c r="E21" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="167">
+        <v>53</v>
+      </c>
+      <c r="F21" s="163">
         <v>12.0</v>
       </c>
-      <c r="G21" s="168"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="174"/>
+      <c r="G21" s="164"/>
+      <c r="H21" s="169"/>
+      <c r="I21" s="170"/>
       <c r="J21" s="63"/>
       <c r="K21" s="63"/>
       <c r="M21" s="32"/>
@@ -2628,17 +2621,17 @@
       <c r="O21" s="32"/>
     </row>
     <row r="22" spans="1:33" customHeight="1" ht="18">
-      <c r="A22" s="166" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="166"/>
+      <c r="A22" s="162" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="162"/>
       <c r="C22" s="57">
         <v>12.0</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="167"/>
-      <c r="G22" s="168"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="164"/>
       <c r="H22" s="3"/>
       <c r="I22" s="4"/>
       <c r="J22" s="42"/>
@@ -2648,19 +2641,19 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:33" customHeight="1" ht="18">
-      <c r="A23" s="166" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="166"/>
+      <c r="A23" s="162" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="162"/>
       <c r="C23" s="57">
         <v>12</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="24"/>
-      <c r="F23" s="167"/>
-      <c r="G23" s="168"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="164"/>
       <c r="H23" s="64" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I23" s="64"/>
       <c r="J23" s="42"/>
@@ -2670,19 +2663,19 @@
       <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:33" customHeight="1" ht="24.75">
-      <c r="A24" s="169" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="169"/>
+      <c r="A24" s="165" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="165"/>
       <c r="C24" s="57"/>
-      <c r="D24" s="170" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="170"/>
-      <c r="F24" s="167"/>
-      <c r="G24" s="168"/>
+      <c r="D24" s="166" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="166"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="164"/>
       <c r="H24" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="65"/>
@@ -2691,15 +2684,15 @@
       <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:33">
-      <c r="A25" s="158" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="159"/>
+      <c r="A25" s="154" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="155"/>
       <c r="C25" s="66"/>
       <c r="D25" s="66"/>
       <c r="E25" s="66"/>
-      <c r="F25" s="162"/>
-      <c r="G25" s="163"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="159"/>
       <c r="H25" s="67"/>
       <c r="I25" s="68"/>
       <c r="J25" s="69"/>
@@ -2709,23 +2702,23 @@
       <c r="O25" s="70"/>
     </row>
     <row r="26" spans="1:33" customHeight="1" ht="13">
-      <c r="A26" s="160"/>
-      <c r="B26" s="161"/>
+      <c r="A26" s="156"/>
+      <c r="B26" s="157"/>
       <c r="C26" s="71" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26" s="72" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="164" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="165"/>
+      <c r="F26" s="160" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="161"/>
       <c r="H26" s="73" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I26" s="74"/>
       <c r="J26" s="31"/>
@@ -2736,7 +2729,7 @@
     </row>
     <row r="27" spans="1:33" customHeight="1" ht="15">
       <c r="C27" s="75" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D27" s="76"/>
       <c r="E27" s="76"/>
@@ -2745,30 +2738,30 @@
       <c r="H27" s="76"/>
     </row>
     <row r="28" spans="1:33" customHeight="1" ht="13.5">
-      <c r="H28" s="154" t="s">
-        <v>66</v>
-      </c>
-      <c r="I28" s="155"/>
+      <c r="H28" s="150" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="151"/>
     </row>
     <row r="29" spans="1:33" customHeight="1" ht="13">
-      <c r="A29" s="156" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="157"/>
+      <c r="A29" s="152" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="153"/>
       <c r="C29" s="77" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D29" s="78"/>
       <c r="E29" s="79" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F29" s="79"/>
       <c r="G29" s="79"/>
       <c r="H29" s="80" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I29" s="81" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M29" s="70"/>
       <c r="N29" s="82"/>
@@ -2778,19 +2771,19 @@
       <c r="AG29" s="16"/>
     </row>
     <row r="30" spans="1:33" customHeight="1" ht="18">
-      <c r="A30" s="136" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="137"/>
+      <c r="A30" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="136"/>
       <c r="C30" s="83">
         <v>5369</v>
       </c>
-      <c r="D30" s="151" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="152"/>
-      <c r="F30" s="152"/>
-      <c r="G30" s="153"/>
+      <c r="D30" s="147" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
+      <c r="G30" s="149"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7">
         <v>1</v>
@@ -2806,27 +2799,27 @@
       </c>
       <c r="O30" s="82"/>
       <c r="Q30" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R30" s="84" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AE30" s="70"/>
       <c r="AF30" s="70"/>
       <c r="AG30" s="70"/>
     </row>
     <row r="31" spans="1:33" customHeight="1" ht="18">
-      <c r="A31" s="136" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="137"/>
+      <c r="A31" s="135" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="136"/>
       <c r="C31" s="83" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="151"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="153"/>
+        <v>77</v>
+      </c>
+      <c r="D31" s="147"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7">
         <v>1</v>
@@ -2840,29 +2833,29 @@
       <c r="N31" s="82"/>
       <c r="O31" s="82"/>
       <c r="Q31" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R31" s="84" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AE31" s="70"/>
       <c r="AF31" s="70"/>
       <c r="AG31" s="70"/>
     </row>
     <row r="32" spans="1:33" customHeight="1" ht="18">
-      <c r="A32" s="136" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="137"/>
+      <c r="A32" s="135" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="136"/>
       <c r="C32" s="85" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="151" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="153"/>
+      <c r="D32" s="147" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="148"/>
+      <c r="F32" s="148"/>
+      <c r="G32" s="149"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7">
         <v>1</v>
@@ -2876,10 +2869,10 @@
       <c r="N32" s="82"/>
       <c r="O32" s="82"/>
       <c r="Q32" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R32" s="84" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE32" s="70">
         <f>H14</f>
@@ -2894,19 +2887,19 @@
       </c>
     </row>
     <row r="33" spans="1:33" customHeight="1" ht="18">
-      <c r="A33" s="136" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="137"/>
+      <c r="A33" s="135" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="136"/>
       <c r="C33" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="E33" s="152"/>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
+      <c r="D33" s="147" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="148"/>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7">
         <v>1</v>
@@ -2922,7 +2915,7 @@
       </c>
       <c r="O33" s="82"/>
       <c r="Q33" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="R33" s="86"/>
       <c r="AE33" s="70">
@@ -2938,15 +2931,20 @@
       </c>
     </row>
     <row r="34" spans="1:33" customHeight="1" ht="18">
-      <c r="A34" s="136" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="137"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="151"/>
-      <c r="E34" s="152"/>
-      <c r="F34" s="152"/>
-      <c r="G34" s="153"/>
+      <c r="A34" s="135" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="136"/>
+      <c r="C34" s="188" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="189" t="str">
+        <f>C11</f>
+        <v>CS19SASHI</v>
+      </c>
+      <c r="E34" s="148"/>
+      <c r="F34" s="148"/>
+      <c r="G34" s="149"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="69"/>
@@ -2955,10 +2953,10 @@
       <c r="N34" s="82"/>
       <c r="O34" s="82"/>
       <c r="Q34" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="R34" s="87" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AA34" s="70">
         <v>6</v>
@@ -2983,19 +2981,19 @@
       </c>
     </row>
     <row r="35" spans="1:33" customHeight="1" ht="18">
-      <c r="A35" s="143" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="144"/>
+      <c r="A35" s="142" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="143"/>
       <c r="C35" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="145" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="146"/>
-      <c r="F35" s="146"/>
-      <c r="G35" s="147"/>
+        <v>90</v>
+      </c>
+      <c r="D35" s="144" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="146"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7">
         <v>1</v>
@@ -3008,10 +3006,10 @@
       <c r="N35" s="82"/>
       <c r="O35" s="82"/>
       <c r="Q35" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R35" s="84" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AA35" s="70">
         <f>AA34</f>
@@ -3029,19 +3027,19 @@
       <c r="AG35" s="82"/>
     </row>
     <row r="36" spans="1:33" customHeight="1" ht="18">
-      <c r="A36" s="136" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="137"/>
+      <c r="A36" s="135" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="136"/>
       <c r="C36" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="145" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="146"/>
-      <c r="F36" s="146"/>
-      <c r="G36" s="147"/>
+        <v>94</v>
+      </c>
+      <c r="D36" s="144" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="145"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="146"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7">
         <v>1</v>
@@ -3054,10 +3052,10 @@
       <c r="N36" s="82"/>
       <c r="O36" s="82"/>
       <c r="Q36" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R36" s="84" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AA36" s="70">
         <v>6</v>
@@ -3074,21 +3072,18 @@
       <c r="AG36" s="82"/>
     </row>
     <row r="37" spans="1:33" customHeight="1" ht="18">
-      <c r="A37" s="136" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" s="137"/>
+      <c r="A37" s="135" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="136"/>
       <c r="C37" s="8" t="str">
         <f>C20</f>
         <v>CS19SASHI</v>
       </c>
-      <c r="D37" s="148" t="str">
-        <f>C21</f>
-        <v>CS 2019 SA SHIRAZ</v>
-      </c>
-      <c r="E37" s="149"/>
-      <c r="F37" s="149"/>
-      <c r="G37" s="150"/>
+      <c r="D37" s="189"/>
+      <c r="E37" s="148"/>
+      <c r="F37" s="148"/>
+      <c r="G37" s="149"/>
       <c r="H37" s="90"/>
       <c r="I37" s="91"/>
       <c r="J37" s="69"/>
@@ -3102,7 +3097,7 @@
       </c>
       <c r="O37" s="82"/>
       <c r="Q37" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R37" s="92"/>
       <c r="AA37" s="70"/>
@@ -3120,15 +3115,15 @@
       </c>
     </row>
     <row r="38" spans="1:33" customHeight="1" ht="24.75">
-      <c r="A38" s="136" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="137"/>
+      <c r="A38" s="135" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="136"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="138"/>
-      <c r="E38" s="139"/>
-      <c r="F38" s="139"/>
-      <c r="G38" s="140"/>
+      <c r="D38" s="137"/>
+      <c r="E38" s="138"/>
+      <c r="F38" s="138"/>
+      <c r="G38" s="139"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="69"/>
@@ -3137,10 +3132,10 @@
       <c r="N38" s="70"/>
       <c r="O38" s="70"/>
       <c r="P38" s="13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AA38" s="70"/>
       <c r="AB38" s="82"/>
@@ -3157,18 +3152,18 @@
       </c>
     </row>
     <row r="39" spans="1:33" customHeight="1" ht="14.9">
-      <c r="A39" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="141"/>
-      <c r="C39" s="141"/>
-      <c r="D39" s="93" t="str">
+      <c r="A39" s="140" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="140"/>
+      <c r="C39" s="140"/>
+      <c r="D39" s="189" t="str">
         <f>C11</f>
         <v>CS19SASHI</v>
       </c>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
+      <c r="E39" s="148"/>
+      <c r="F39" s="148"/>
+      <c r="G39" s="149"/>
       <c r="H39" s="24"/>
       <c r="J39" s="42"/>
       <c r="K39" s="42"/>
@@ -3197,12 +3192,12 @@
       </c>
     </row>
     <row r="40" spans="1:33" customHeight="1" ht="13">
-      <c r="A40" s="129" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="129"/>
-      <c r="C40" s="95">
-        <v>0</v>
+      <c r="A40" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="128"/>
+      <c r="C40" s="94" t="s">
+        <v>40</v>
       </c>
       <c r="D40" s="24"/>
       <c r="J40" s="42"/>
@@ -3225,14 +3220,14 @@
       <c r="AG40" s="82"/>
     </row>
     <row r="41" spans="1:33" customHeight="1" ht="13">
-      <c r="A41" s="129" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="129"/>
+      <c r="A41" s="128" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="128"/>
       <c r="C41" s="93" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="95"/>
+        <v>103</v>
+      </c>
+      <c r="D41" s="94"/>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
       <c r="G41" s="31"/>
@@ -3257,20 +3252,20 @@
       <c r="AG41" s="70"/>
     </row>
     <row r="42" spans="1:33" customHeight="1" ht="13">
-      <c r="A42" s="129" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="129"/>
+      <c r="A42" s="128" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="128"/>
       <c r="C42" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E42" s="96" t="s">
-        <v>105</v>
-      </c>
-      <c r="F42" s="97"/>
+        <v>106</v>
+      </c>
+      <c r="E42" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" s="96"/>
       <c r="J42" s="42"/>
       <c r="K42" s="42"/>
       <c r="M42" s="70"/>
@@ -3287,15 +3282,15 @@
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="98" t="s">
-        <v>104</v>
-      </c>
-      <c r="E43" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" s="99"/>
+      <c r="E43" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43" s="98"/>
       <c r="J43" s="42"/>
       <c r="K43" s="42"/>
       <c r="M43" s="70"/>
@@ -3312,15 +3307,15 @@
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="98" t="s">
-        <v>104</v>
-      </c>
-      <c r="E44" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" s="99"/>
+        <v>110</v>
+      </c>
+      <c r="D44" s="97" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="98"/>
       <c r="J44" s="42"/>
       <c r="K44" s="42"/>
       <c r="M44" s="70"/>
@@ -3337,12 +3332,12 @@
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="100"/>
-      <c r="E45" s="99"/>
-      <c r="F45" s="99"/>
-      <c r="H45" s="101"/>
+        <v>111</v>
+      </c>
+      <c r="D45" s="99"/>
+      <c r="E45" s="98"/>
+      <c r="F45" s="98"/>
+      <c r="H45" s="100"/>
       <c r="M45" s="70"/>
       <c r="N45" s="70"/>
       <c r="O45" s="70"/>
@@ -3354,10 +3349,10 @@
       <c r="AG45" s="70"/>
     </row>
     <row r="46" spans="1:33" customHeight="1" ht="13">
-      <c r="A46" s="102" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" s="102"/>
+      <c r="A46" s="101" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="101"/>
       <c r="C46" s="16"/>
       <c r="H46" s="16"/>
       <c r="M46" s="70"/>
@@ -3371,10 +3366,10 @@
       <c r="AG46" s="70"/>
     </row>
     <row r="47" spans="1:33" customHeight="1" ht="9">
-      <c r="A47" s="102"/>
-      <c r="B47" s="102"/>
+      <c r="A47" s="101"/>
+      <c r="B47" s="101"/>
       <c r="C47" s="16"/>
-      <c r="D47" s="99"/>
+      <c r="D47" s="98"/>
       <c r="H47" s="16"/>
       <c r="M47" s="70"/>
       <c r="N47" s="70"/>
@@ -3387,25 +3382,25 @@
       <c r="AG47" s="70"/>
     </row>
     <row r="48" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A48" s="129" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" s="129"/>
-      <c r="C48" s="142" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="142"/>
-      <c r="E48" s="103" t="s">
-        <v>112</v>
-      </c>
-      <c r="G48" s="104" t="s">
+      <c r="A48" s="128" t="s">
         <v>113</v>
       </c>
+      <c r="B48" s="128"/>
+      <c r="C48" s="141" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="141"/>
+      <c r="E48" s="102" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="103" t="s">
+        <v>115</v>
+      </c>
       <c r="H48" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I48" s="105" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="I48" s="104" t="s">
+        <v>117</v>
       </c>
       <c r="J48" s="42"/>
       <c r="K48" s="42"/>
@@ -3420,17 +3415,23 @@
       <c r="AG48" s="70"/>
     </row>
     <row r="49" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A49" s="129" t="s">
-        <v>116</v>
-      </c>
-      <c r="B49" s="129"/>
-      <c r="C49" s="106"/>
-      <c r="D49" s="106"/>
-      <c r="E49" s="103"/>
+      <c r="A49" s="128" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="128"/>
+      <c r="C49" s="105">
+        <v>29</v>
+      </c>
+      <c r="D49" s="105">
+        <v>28</v>
+      </c>
+      <c r="E49" s="102">
+        <v>100</v>
+      </c>
       <c r="H49" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I49" s="107"/>
+        <v>119</v>
+      </c>
+      <c r="I49" s="106"/>
       <c r="J49" s="42"/>
       <c r="K49" s="42"/>
       <c r="M49" s="70"/>
@@ -3444,17 +3445,23 @@
       <c r="AG49" s="70"/>
     </row>
     <row r="50" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A50" s="129" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" s="129"/>
-      <c r="C50" s="106"/>
-      <c r="D50" s="106"/>
-      <c r="E50" s="103"/>
+      <c r="A50" s="128" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="128"/>
+      <c r="C50" s="105">
+        <v>4</v>
+      </c>
+      <c r="D50" s="105">
+        <v>4</v>
+      </c>
+      <c r="E50" s="102">
+        <v>10</v>
+      </c>
       <c r="H50" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="I50" s="107"/>
+        <v>121</v>
+      </c>
+      <c r="I50" s="106"/>
       <c r="J50" s="42"/>
       <c r="K50" s="42"/>
       <c r="AA50" s="70"/>
@@ -3465,14 +3472,20 @@
       <c r="AG50" s="70"/>
     </row>
     <row r="51" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A51" s="129" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" s="129"/>
-      <c r="C51" s="106"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="103"/>
-      <c r="I51" s="108"/>
+      <c r="A51" s="128" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" s="128"/>
+      <c r="C51" s="105">
+        <v>116</v>
+      </c>
+      <c r="D51" s="105">
+        <v>112</v>
+      </c>
+      <c r="E51" s="102">
+        <v>1000</v>
+      </c>
+      <c r="I51" s="107"/>
       <c r="J51" s="42"/>
       <c r="K51" s="42"/>
       <c r="M51" s="70"/>
@@ -3486,28 +3499,28 @@
       <c r="AG51" s="70"/>
     </row>
     <row r="52" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A52" s="129" t="s">
-        <v>121</v>
-      </c>
-      <c r="B52" s="129"/>
-      <c r="C52" s="135" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52" s="135"/>
-      <c r="G52" s="104" t="s">
-        <v>122</v>
+      <c r="A52" s="128" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="128"/>
+      <c r="C52" s="134" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="134"/>
+      <c r="G52" s="103" t="s">
+        <v>124</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I52" s="109" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="I52" s="108" t="s">
+        <v>117</v>
       </c>
       <c r="J52" s="42"/>
       <c r="K52" s="42"/>
       <c r="M52" s="70">
         <f>C51</f>
-        <v/>
+        <v>116</v>
       </c>
       <c r="N52" s="70"/>
       <c r="O52" s="82"/>
@@ -3519,18 +3532,18 @@
       <c r="AG52" s="70"/>
     </row>
     <row r="53" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A53" s="132" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="132"/>
-      <c r="C53" s="133" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="133"/>
+      <c r="A53" s="131" t="s">
+        <v>125</v>
+      </c>
+      <c r="B53" s="131"/>
+      <c r="C53" s="132" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="132"/>
       <c r="H53" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I53" s="109"/>
+        <v>119</v>
+      </c>
+      <c r="I53" s="108"/>
       <c r="J53" s="42"/>
       <c r="K53" s="42"/>
       <c r="M53" s="70"/>
@@ -3541,32 +3554,32 @@
       <c r="AC53" s="70"/>
       <c r="AE53" s="70">
         <f>C51</f>
-        <v/>
+        <v>116</v>
       </c>
       <c r="AF53" s="70">
         <v>2.5</v>
       </c>
-      <c r="AG53" s="70" t="e">
+      <c r="AG53" s="70">
         <f>AF53/AE53</f>
-        <v>#DIV/0!</v>
+        <v>0.021551724137931</v>
       </c>
     </row>
     <row r="54" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A54" s="129" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="129"/>
-      <c r="C54" s="133" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="133"/>
+      <c r="A54" s="128" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="128"/>
+      <c r="C54" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="D54" s="132"/>
       <c r="H54" s="10"/>
-      <c r="I54" s="108"/>
+      <c r="I54" s="107"/>
       <c r="J54" s="42"/>
       <c r="K54" s="42"/>
       <c r="M54" s="70">
         <f>M52</f>
-        <v/>
+        <v>116</v>
       </c>
       <c r="N54" s="70"/>
       <c r="O54" s="82"/>
@@ -3578,16 +3591,16 @@
       <c r="AG54" s="70"/>
     </row>
     <row r="55" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A55" s="129" t="s">
-        <v>126</v>
-      </c>
-      <c r="B55" s="129"/>
-      <c r="C55" s="134" t="s">
-        <v>127</v>
-      </c>
-      <c r="D55" s="134"/>
+      <c r="A55" s="128" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="128"/>
+      <c r="C55" s="133" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="133"/>
       <c r="H55" s="10"/>
-      <c r="I55" s="108"/>
+      <c r="I55" s="107"/>
       <c r="J55" s="42"/>
       <c r="K55" s="42"/>
       <c r="M55" s="70"/>
@@ -3601,12 +3614,12 @@
       <c r="AG55" s="70"/>
     </row>
     <row r="56" spans="1:33" customHeight="1" ht="13">
-      <c r="A56" s="129" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" s="129"/>
-      <c r="C56" s="130"/>
-      <c r="D56" s="130"/>
+      <c r="A56" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" s="128"/>
+      <c r="C56" s="129"/>
+      <c r="D56" s="129"/>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
@@ -3624,10 +3637,10 @@
       <c r="AG56" s="82"/>
     </row>
     <row r="57" spans="1:33" customHeight="1" ht="13">
-      <c r="A57" s="129" t="s">
-        <v>129</v>
-      </c>
-      <c r="B57" s="129"/>
+      <c r="A57" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="128"/>
       <c r="C57" s="34"/>
       <c r="D57" s="34"/>
       <c r="E57" s="34"/>
@@ -3653,10 +3666,10 @@
     </row>
     <row r="58" spans="1:33">
       <c r="K58" s="31"/>
-      <c r="M58" s="110" t="s">
-        <v>130</v>
-      </c>
-      <c r="N58" s="111"/>
+      <c r="M58" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="N58" s="110"/>
       <c r="O58" s="82"/>
       <c r="AA58" s="70"/>
       <c r="AB58" s="82"/>
@@ -3666,130 +3679,130 @@
       <c r="AG58" s="70"/>
     </row>
     <row r="59" spans="1:33" customHeight="1" ht="15.75">
-      <c r="A59" s="127" t="s">
-        <v>131</v>
-      </c>
-      <c r="B59" s="127"/>
-      <c r="C59" s="131"/>
-      <c r="D59" s="131"/>
-      <c r="E59" s="131"/>
-      <c r="F59" s="127" t="s">
-        <v>132</v>
-      </c>
-      <c r="G59" s="127"/>
-      <c r="H59" s="112"/>
-      <c r="I59" s="113"/>
-      <c r="J59" s="113"/>
-      <c r="K59" s="114"/>
+      <c r="A59" s="126" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="126"/>
+      <c r="C59" s="130"/>
+      <c r="D59" s="130"/>
+      <c r="E59" s="130"/>
+      <c r="F59" s="126" t="s">
+        <v>134</v>
+      </c>
+      <c r="G59" s="126"/>
+      <c r="H59" s="111"/>
+      <c r="I59" s="112"/>
+      <c r="J59" s="112"/>
+      <c r="K59" s="113"/>
       <c r="M59" s="70" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="N59" s="70"/>
       <c r="O59" s="82"/>
     </row>
     <row r="60" spans="1:33" customHeight="1" ht="15.5">
-      <c r="A60" s="115"/>
-      <c r="B60" s="115"/>
-      <c r="Q60" s="116"/>
-      <c r="AA60" s="117"/>
-      <c r="AB60" s="118"/>
-      <c r="AC60" s="118"/>
-      <c r="AE60" s="117"/>
-      <c r="AF60" s="117"/>
-      <c r="AG60" s="117"/>
+      <c r="A60" s="114"/>
+      <c r="B60" s="114"/>
+      <c r="Q60" s="115"/>
+      <c r="AA60" s="116"/>
+      <c r="AB60" s="117"/>
+      <c r="AC60" s="117"/>
+      <c r="AE60" s="116"/>
+      <c r="AF60" s="116"/>
+      <c r="AG60" s="116"/>
     </row>
     <row r="61" spans="1:33" customHeight="1" ht="21.75">
-      <c r="A61" s="127"/>
-      <c r="B61" s="127"/>
-      <c r="C61" s="128"/>
-      <c r="D61" s="128"/>
-      <c r="E61" s="128"/>
-      <c r="F61" s="127"/>
-      <c r="G61" s="127"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="120"/>
-      <c r="J61" s="120"/>
-      <c r="K61" s="114"/>
-      <c r="L61" s="114"/>
-      <c r="M61" s="114"/>
-      <c r="N61" s="114"/>
-      <c r="O61" s="114"/>
-      <c r="P61" s="114"/>
-      <c r="AA61" s="117"/>
-      <c r="AB61" s="117"/>
-      <c r="AC61" s="117"/>
-      <c r="AE61" s="117"/>
-      <c r="AF61" s="117"/>
-      <c r="AG61" s="117"/>
+      <c r="A61" s="126"/>
+      <c r="B61" s="126"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="127"/>
+      <c r="E61" s="127"/>
+      <c r="F61" s="126"/>
+      <c r="G61" s="126"/>
+      <c r="H61" s="118"/>
+      <c r="I61" s="119"/>
+      <c r="J61" s="119"/>
+      <c r="K61" s="113"/>
+      <c r="L61" s="113"/>
+      <c r="M61" s="113"/>
+      <c r="N61" s="113"/>
+      <c r="O61" s="113"/>
+      <c r="P61" s="113"/>
+      <c r="AA61" s="116"/>
+      <c r="AB61" s="116"/>
+      <c r="AC61" s="116"/>
+      <c r="AE61" s="116"/>
+      <c r="AF61" s="116"/>
+      <c r="AG61" s="116"/>
     </row>
     <row r="62" spans="1:33" customHeight="1" ht="3">
-      <c r="A62" s="121"/>
-      <c r="B62" s="121"/>
-      <c r="C62" s="121"/>
-      <c r="D62" s="122"/>
-      <c r="E62" s="122"/>
-      <c r="F62" s="122"/>
-      <c r="G62" s="122"/>
-      <c r="H62" s="123"/>
-      <c r="I62" s="122"/>
-      <c r="J62" s="122"/>
-      <c r="K62" s="114"/>
-      <c r="L62" s="114"/>
-      <c r="M62" s="114"/>
-      <c r="N62" s="114"/>
-      <c r="O62" s="114"/>
-      <c r="P62" s="114"/>
-      <c r="AA62" s="117"/>
-      <c r="AB62" s="117"/>
-      <c r="AC62" s="117"/>
-      <c r="AE62" s="117"/>
-      <c r="AF62" s="117"/>
-      <c r="AG62" s="117"/>
+      <c r="A62" s="120"/>
+      <c r="B62" s="120"/>
+      <c r="C62" s="120"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="121"/>
+      <c r="F62" s="121"/>
+      <c r="G62" s="121"/>
+      <c r="H62" s="122"/>
+      <c r="I62" s="121"/>
+      <c r="J62" s="121"/>
+      <c r="K62" s="113"/>
+      <c r="L62" s="113"/>
+      <c r="M62" s="113"/>
+      <c r="N62" s="113"/>
+      <c r="O62" s="113"/>
+      <c r="P62" s="113"/>
+      <c r="AA62" s="116"/>
+      <c r="AB62" s="116"/>
+      <c r="AC62" s="116"/>
+      <c r="AE62" s="116"/>
+      <c r="AF62" s="116"/>
+      <c r="AG62" s="116"/>
     </row>
     <row r="63" spans="1:33" customHeight="1" ht="14.5">
-      <c r="A63" s="124"/>
-      <c r="B63" s="124"/>
-      <c r="C63" s="124"/>
-      <c r="D63" s="124"/>
-      <c r="E63" s="101"/>
-      <c r="F63" s="101"/>
-      <c r="G63" s="124"/>
-      <c r="H63" s="124"/>
-      <c r="I63" s="124"/>
-      <c r="J63" s="125"/>
-      <c r="K63" s="125"/>
+      <c r="A63" s="123"/>
+      <c r="B63" s="123"/>
+      <c r="C63" s="123"/>
+      <c r="D63" s="123"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="100"/>
+      <c r="G63" s="123"/>
+      <c r="H63" s="123"/>
+      <c r="I63" s="123"/>
+      <c r="J63" s="124"/>
+      <c r="K63" s="124"/>
     </row>
     <row r="64" spans="1:33" customHeight="1" ht="14.5">
-      <c r="A64" s="124"/>
-      <c r="B64" s="124"/>
-      <c r="C64" s="124"/>
-      <c r="D64" s="124"/>
-      <c r="E64" s="101"/>
-      <c r="F64" s="101"/>
-      <c r="G64" s="124"/>
-      <c r="H64" s="124"/>
-      <c r="I64" s="124"/>
-      <c r="J64" s="125"/>
-      <c r="K64" s="125"/>
+      <c r="A64" s="123"/>
+      <c r="B64" s="123"/>
+      <c r="C64" s="123"/>
+      <c r="D64" s="123"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="100"/>
+      <c r="G64" s="123"/>
+      <c r="H64" s="123"/>
+      <c r="I64" s="123"/>
+      <c r="J64" s="124"/>
+      <c r="K64" s="124"/>
     </row>
     <row r="65" spans="1:33" customHeight="1" ht="14.5">
-      <c r="A65" s="124"/>
-      <c r="B65" s="124"/>
-      <c r="C65" s="124"/>
-      <c r="D65" s="124"/>
-      <c r="E65" s="101"/>
-      <c r="F65" s="101"/>
-      <c r="G65" s="124"/>
-      <c r="H65" s="124"/>
-      <c r="I65" s="124"/>
-      <c r="J65" s="125"/>
-      <c r="K65" s="125"/>
+      <c r="A65" s="123"/>
+      <c r="B65" s="123"/>
+      <c r="C65" s="123"/>
+      <c r="D65" s="123"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
+      <c r="G65" s="123"/>
+      <c r="H65" s="123"/>
+      <c r="I65" s="123"/>
+      <c r="J65" s="124"/>
+      <c r="K65" s="124"/>
     </row>
     <row r="66" spans="1:33" customHeight="1" ht="13">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
     </row>
-    <row r="123" spans="1:33" customHeight="1" ht="14.5" s="126" customFormat="1"/>
+    <row r="123" spans="1:33" customHeight="1" ht="14.5" s="125" customFormat="1"/>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
@@ -3857,6 +3870,7 @@
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D39:G39"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="A54:B54"/>
@@ -3938,6 +3952,16 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D37:G37">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39:G39">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId_hyperlink_1"/>
   </hyperlinks>
@@ -3971,7 +3995,7 @@
   <sheetData>
     <row r="3" spans="1:2" customHeight="1" ht="14.5">
       <c r="B3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>